<commit_message>
TestScript for DataDriven AddCarrier - WovenWrap
</commit_message>
<xml_diff>
--- a/TestData/Testdata_add_woven_wrap.xlsx
+++ b/TestData/Testdata_add_woven_wrap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WrapTrack.Stf\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E7D8A59F-09AB-4838-A69F-B457A0CA704D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B79A89E-DD61-4778-B8E4-F2F143379CBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{DD668BB2-894F-4898-8D1A-BC998BBD9F5D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>Woven wrap</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Acquired</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>Home made</t>
   </si>
   <si>
@@ -69,15 +66,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>"MyOwn_"+datoTid</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>dd - 1 d</t>
-  </si>
-  <si>
     <t>dd - 3 d</t>
   </si>
   <si>
@@ -93,12 +81,6 @@
     <t>dd + 3 d</t>
   </si>
   <si>
-    <t>dd - 1y</t>
-  </si>
-  <si>
-    <t>dd - 2 y</t>
-  </si>
-  <si>
     <t>A Love So Rare</t>
   </si>
   <si>
@@ -157,6 +139,27 @@
   </si>
   <si>
     <t>CarrierType</t>
+  </si>
+  <si>
+    <t>{TODAY}</t>
+  </si>
+  <si>
+    <t>MyOwn_{TODAY}{NOW}</t>
+  </si>
+  <si>
+    <t>{TODAY - 1 day}</t>
+  </si>
+  <si>
+    <t>{TODAY - 1 year}</t>
+  </si>
+  <si>
+    <t>{TODAY - 2 year}</t>
+  </si>
+  <si>
+    <t>StfIgnoreRow</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -227,9 +230,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -267,7 +270,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -373,7 +376,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -523,14 +526,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87EC161-FA34-4330-9424-68515F7DC37B}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
@@ -541,17 +545,17 @@
     <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -566,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -584,13 +588,19 @@
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -601,24 +611,27 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J3">
         <v>8</v>
@@ -627,21 +640,24 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J4">
         <v>7</v>
@@ -650,30 +666,33 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="b">
+        <v>0</v>
+      </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
         <v>1975</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="J5">
         <v>6</v>
@@ -682,27 +701,30 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="b">
+        <v>0</v>
+      </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J6">
         <v>5</v>
@@ -711,21 +733,24 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J7">
         <v>4</v>
@@ -734,33 +759,36 @@
         <v>3</v>
       </c>
       <c r="L7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="I8" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" t="s">
-        <v>33</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -769,33 +797,36 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="b">
+        <v>0</v>
+      </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2">
         <v>1975</v>
       </c>
       <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" t="s">
-        <v>36</v>
-      </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -804,27 +835,30 @@
         <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -833,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>